<commit_message>
delete unncessary scripts, add argument desc in functions
</commit_message>
<xml_diff>
--- a/model_settings.xlsx
+++ b/model_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rde/Net/Groups/BGI/people/rde/Models/02_Mengoli_PModel/06_MS_02_VariationInParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A9C517-2A5E-0843-963B-8F1FDEFDBD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A14AAD-D8A8-3540-BCC7-55A46D4B4F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="22100" windowWidth="26660" windowHeight="17500" xr2:uid="{5FCEDB57-C8D2-3444-B5A2-2B7A440EDA96}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>How to filter data</t>
   </si>
   <si>
-    <t>estimate parameters per site, per site year, per PFT, global for all sites</t>
-  </si>
-  <si>
     <t>model_name</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>optim</t>
   </si>
   <si>
-    <t>site_year</t>
-  </si>
-  <si>
     <t>sequence</t>
   </si>
   <si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>The group of parameters which will vary per year, while other parameters will remain fixed. (only Group 1-4 should be selected for P-model, for LUE model Group 1-8 can be selected).</t>
+  </si>
+  <si>
+    <t>all_year</t>
+  </si>
+  <si>
+    <t>estimate parameters per site, per site year, per PFT, global for all sites; all_sites must be selected for the experiment in which a group of param vary per year, while other param are fixed across years.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -582,18 +582,18 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.2">
@@ -601,21 +601,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="144" x14ac:dyDescent="0.25">
@@ -623,21 +623,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -678,21 +678,21 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.2">
@@ -700,32 +700,32 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="72" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean forward run codes
</commit_message>
<xml_diff>
--- a/model_settings.xlsx
+++ b/model_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rde/Net/Groups/BGI/people/rde/Models/02_Mengoli_PModel/06_MS_02_VariationInParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A14AAD-D8A8-3540-BCC7-55A46D4B4F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9471BCB6-6BBA-B64E-9C5F-1E620CF74703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="22100" windowWidth="26660" windowHeight="17500" xr2:uid="{5FCEDB57-C8D2-3444-B5A2-2B7A440EDA96}"/>
   </bookViews>
@@ -162,7 +162,7 @@
     <t>all_year</t>
   </si>
   <si>
-    <t>estimate parameters per site, per site year, per PFT, global for all sites; all_sites must be selected for the experiment in which a group of param vary per year, while other param are fixed across years.</t>
+    <t>only `all_sites` must be selected. This settings file to be used for the experiment in which a group of param vary per year, while other param are fixed across years.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,15 +729,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{751F1F23-705C-A045-87E9-6995A7AB99B3}">
       <formula1>"BRK15"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{3C87A5E6-4FD5-064E-B78C-16F49C8BA313}">
       <formula1>"optim, forward"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{50498385-B434-0843-A7D4-DB832D42104E}">
-      <formula1>"all_year, site_year, per_pft, global_opti"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{4781B7A3-6256-024D-800A-2BAF0EBAF3BB}">
       <formula1>"sequence, parallel, summarize_exp_results"</formula1>

</xml_diff>

<commit_message>
update model settings option
</commit_message>
<xml_diff>
--- a/model_settings.xlsx
+++ b/model_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rde/Net/Groups/BGI/people/rde/Models/02_Mengoli_PModel/06_MS_02_VariationInParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9471BCB6-6BBA-B64E-9C5F-1E620CF74703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C97A16F-ED43-FF4E-9CDD-6A65C4ACAFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="22100" windowWidth="26660" windowHeight="17500" xr2:uid="{5FCEDB57-C8D2-3444-B5A2-2B7A440EDA96}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>ip_data_path</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>only `all_sites` must be selected. This settings file to be used for the experiment in which a group of param vary per year, while other param are fixed across years.</t>
+  </si>
+  <si>
+    <t>et_var_name</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Choose between which variable to use for ET. ET is based on LE. ET_CORR is based energy-balance corrected (as done in OneFlux) LE_CORR variable</t>
   </si>
 </sst>
 </file>
@@ -550,10 +559,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2062C1B3-0EC7-0940-8796-9CF8D94A4E67}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,8 +737,23 @@
         <v>40</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5"/>
+    </row>
   </sheetData>
-  <dataValidations count="11">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{751F1F23-705C-A045-87E9-6995A7AB99B3}">
       <formula1>"BRK15"</formula1>
     </dataValidation>
@@ -762,6 +786,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{3EAC1951-D840-6C40-A5F7-2CEE50C6E691}">
       <formula1>"Group1,Group2,Group3,Group4,Group5,Group6,Group7,Group8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{F7DC07A1-39BA-B64D-BCC6-F8F55E75935D}">
+      <formula1>"ET, ET_CORR"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>